<commit_message>
reading metadata for library
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,44 +434,29 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Subcategory</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Sheet name</t>
+          <t>sheet_name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Sort priority</t>
+          <t>category</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Is default subcategory</t>
+          <t>category_name</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Category</t>
+          <t>subcategory_sort_priority</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Category name</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Category priority</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Is default category</t>
+          <t>category_sort_priority</t>
         </is>
       </c>
     </row>
@@ -486,31 +471,21 @@
           <t>Прочее</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Прочее</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Прочие материалы</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
         <v>5</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Прочее</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Прочие материалы</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
+      <c r="F2" t="n">
         <v>3</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
       </c>
     </row>
     <row r="3">
@@ -524,14 +499,22 @@
           <t>Метизы</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Прочее</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Прочие материалы</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>4</v>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -544,14 +527,22 @@
           <t>Метизы 2</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Прочее</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Прочие материалы</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>4</v>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -564,14 +555,22 @@
           <t>Коробки</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Прочее</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Прочие материалы</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>3</v>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -584,14 +583,22 @@
           <t>Трубы</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Прочее</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Прочие материалы</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>2</v>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -604,28 +611,22 @@
           <t>Кабель</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Кабель</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Кабельные изделия</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>1</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Кабель</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Кабельные изделия</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
+      <c r="F7" t="n">
         <v>2</v>
       </c>
-      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -638,28 +639,22 @@
           <t>Светильники</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Свет</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Светотехническое оборудование</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>0</v>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Свет</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Светотехническое оборудование</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
+      <c r="F8" t="n">
         <v>1</v>
       </c>
-      <c r="H8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>